<commit_message>
Booking API - new booking & get bookings | Modified other APIs to accomodate changes with seats
</commit_message>
<xml_diff>
--- a/API_documentation.xlsx
+++ b/API_documentation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhitholar/college_work/cmpe202/ind_project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhitholar/college_work/cmpe202/team_project/team-project-team_techies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2990162C-9842-7C4A-B196-C39B9A48BF77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B37C742-5245-084F-B3D7-33D75F105959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{AB8BB195-AD8F-664F-886C-5E9BDDAF898A}"/>
+    <workbookView xWindow="10640" yWindow="-21100" windowWidth="28800" windowHeight="16240" xr2:uid="{AB8BB195-AD8F-664F-886C-5E9BDDAF898A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
   <si>
     <t>Methid</t>
   </si>
@@ -346,40 +346,129 @@
     </r>
   </si>
   <si>
-    <t>{"flight_id" : "3",
-    "aircraft" : "6184aa07c2bf805a6ec51679",
+    <t>"Flight ID already registered"</t>
+  </si>
+  <si>
+    <t>Response1</t>
+  </si>
+  <si>
+    <t>Response2</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:5000/flight?depart_date=2022-01-06&amp;airport1=61849d5f4367d925b16ff24c&amp;airport2=61849d3f4367d925b16ff24b</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "_id": {
+            "$oid": "61849d3f4367d925b16ff24b"
+        },
+        "city": "San Jose",
+        "code": "SJC",
+        "modified_at": {
+            "$date": 1636055759037
+        },
+        "name": "San Jose International Airport"
+    }]</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Api not used in UI currently</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "_id": {
+            "$oid": "61849d5f4367d925b16ff24c"
+        },
+        "city": "San Francisco",
+        "code": "SFO",
+        "modified_at": {
+            "$date": 1636055791184
+        },
+        "name": "San Francisco International Airport"
+    }
+]</t>
+  </si>
+  <si>
+    <t>Admin required -- backend handled</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://127.0.0.1:5000/airport/61849d5f4367d925b16ff24c</t>
+  </si>
+  <si>
+    <t>{   "flight_num" : "3455",
+    "aircraft" : "6184a9d1c2bf805a6ec5164a",
     "departure_airport" :"61849d5f4367d925b16ff24c",
     "arrival_airport" :"61849d3f4367d925b16ff24b",
     "departure_date": "2022-01-06",
     "arrival_date" : "2022-01-06",
     "departure_time": "10:00",
     "arrival_time":"11:00",
-    "price" : 40,
-    "mileage_points": 4 
+    "price" : 40
 }</t>
   </si>
   <si>
-    <t>"Flight ID already registered"</t>
-  </si>
-  <si>
-    <t>Response1</t>
-  </si>
-  <si>
-    <t>Response2</t>
-  </si>
-  <si>
-    <t>"Flight - AA1234 added successfully"</t>
-  </si>
-  <si>
-    <t>http://127.0.0.1:5000/flight?depart_date=2022-01-06&amp;airport1=61849d5f4367d925b16ff24c&amp;airport2=61849d3f4367d925b16ff24b</t>
+    <t>"Flight - 3455 added successfully"</t>
+  </si>
+  <si>
+    <t>Get Flight by ID</t>
+  </si>
+  <si>
+    <t>/flight/id</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:5000/flight/6192ab07a2728d81e6aa6e11</t>
+  </si>
+  <si>
+    <t>{
+    "_id": {
+        "$oid": "6192ab07a2728d81e6aa6e11"
+    },
+    "aircraft": {
+        "$oid": "6184a9d1c2bf805a6ec5164a"
+    },
+    "arrival_airport": {
+        "$oid": "61849d3f4367d925b16ff24b"
+    },
+    "arrival_date": {
+        "$date": 1641427200000
+    },
+    "arrival_time": "11:00",
+    "departure_airport": {
+        "$oid": "61849d5f4367d925b16ff24c"
+    },
+    "departure_date": {
+        "$date": 1641427200000
+    },
+    "departure_time": "10:00",
+    "flight_num": "AA3455",
+    "flight_status": "scheduled",
+    "mileage_points": 4,
+    "modified_at": {
+        "$date": 1636973191119
+    },
+    "price": 40.0,
+    "remaining_seats": 60,
+    "seats": {
+        "aisle": 20,
+        "middle": 20,
+        "window": 20
+    }
+}</t>
   </si>
   <si>
     <t>[
     {
         "_id": {
-            "$oid": "6184c5f1e0027a37b70b4843"
-        },
-        "aircraft": "/aircraft/6184aa07c2bf805a6ec51679",
+            "$oid": "6192ab07a2728d81e6aa6e11"
+        },
+        "aircraft": "/aircraft/6184a9d1c2bf805a6ec5164a",
         "arrival_airport": "/airport/61849d3f4367d925b16ff24b",
         "arrival_date": {
             "$date": 1641427200000
@@ -390,86 +479,225 @@
             "$date": 1641427200000
         },
         "departure_time": "10:00",
-        "flight_id": "3",
+        "flight_num": "AA3455",
+        "flight_status": "scheduled",
         "mileage_points": 4,
         "modified_at": {
-            "$date": 1636066177110
-        },
-        "price": 40.0
+            "$date": 1636973191119
+        },
+        "price": 40.0,
+        "remaining_seats": 60,
+        "seats": {
+            "aisle": 20,
+            "middle": 20,
+            "window": 20
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>Aircraft</t>
+  </si>
+  <si>
+    <t>/aircraft</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "_id": {
+            "$oid": "6184a9d1c2bf805a6ec5164a"
+        },
+        "name": "Boeing 737",
+        "seats": {
+            "aisle": 20,
+            "middle": 20,
+            "window": 20
+        },
+        "total_seats": 60
     },
     {
         "_id": {
-            "$oid": "618b024f730430b33a9776f9"
-        },
-        "aircraft": "/aircraft/6184aa07c2bf805a6ec51679",
-        "arrival_airport": "/airport/61849d3f4367d925b16ff24b",
-        "arrival_date": {
-            "$date": 1641427200000
-        },
-        "arrival_time": "11:00",
-        "departure_airport": "/airport/61849d5f4367d925b16ff24c",
-        "departure_date": {
-            "$date": 1641427200000
-        },
-        "departure_time": "10:00",
-        "flight_id": "4",
-        "mileage_points": 4,
-        "modified_at": {
-            "$date": 1636471247140
-        },
-        "price": 40.0
-    }]</t>
-  </si>
-  <si>
-    <t>[]</t>
+            "$oid": "6184aa07c2bf805a6ec51679"
+        },
+        "name": "Airbus A320",
+        "seats": {
+            "aisle": 30,
+            "middle": 30,
+            "window": 30
+        },
+        "total_seats": 90
+    }
+]</t>
+  </si>
+  <si>
+    <t>/aircraft/id</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:5000/aircraft/6184aa07c2bf805a6ec51679</t>
+  </si>
+  <si>
+    <t>{
+    "_id": {
+        "$oid": "6184aa07c2bf805a6ec51679"
+    },
+    "name": "Airbus A320",
+    "seats": {
+        "aisle": 30,
+        "middle": 30,
+        "window": 30
+    },
+    "total_seats": 90
+}</t>
+  </si>
+  <si>
+    <t>Add aircraft- Not implemented</t>
+  </si>
+  <si>
+    <t>Get all aircraft</t>
+  </si>
+  <si>
+    <t>Get aircraft by ID</t>
+  </si>
+  <si>
+    <t>Booking</t>
+  </si>
+  <si>
+    <t>Book a flight</t>
+  </si>
+  <si>
+    <t>/booking</t>
+  </si>
+  <si>
+    <t>{
+    "message": "No such Flight exists"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "message": "Booking successful"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "message": "Flight is full"
+}</t>
+  </si>
+  <si>
+    <t>Booking of a customer</t>
+  </si>
+  <si>
+    <t>None, customer id will be taken from jwt by the backend</t>
+  </si>
+  <si>
+    <t>Get booking by id</t>
+  </si>
+  <si>
+    <t>/booking/id</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:5000/booking/6192d0a8f5cb2f59a7dd4b6e</t>
+  </si>
+  <si>
+    <t>{
+    "_id": {
+        "$oid": "6192d0a8f5cb2f59a7dd4b6e"
+    },
+    "booking_history": "booked",
+    "booking_num": "#940QL3FTF99N",
+    "customer_oid": {
+        "$oid": "618176b53dc26f93f1129a9d"
+    },
+    "flight_oid": "/flight/6192c74866cb83011fbe931a",
+    "mileage_points_earned": 4,
+    "modified_at": {
+        "$date": 1636982824139
+    },
+    "seat": "None"
+}</t>
   </si>
   <si>
     <t>[
     {
         "_id": {
-            "$oid": "61849d3f4367d925b16ff24b"
-        },
-        "city": "San Jose",
-        "code": "SJC",
+            "$oid": "6192d0a8f5cb2f59a7dd4b6e"
+        },
+        "booking_history": "booked",
+        "booking_num": "#940QL3FTF99N",
+        "customer_oid": {
+            "$oid": "618176b53dc26f93f1129a9d"
+        },
+        "flight_oid": "/flight/6192c74866cb83011fbe931a",
+        "mileage_points_earned": 4,
         "modified_at": {
-            "$date": 1636055759037
-        },
-        "name": "San Jose International Airport"
-    }]</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Api not used in UI currently</t>
-  </si>
-  <si>
-    <t>URL sent by backend: http://127.0.0.1:5000/airport/61849d5f4367d925b16ff24c</t>
-  </si>
-  <si>
-    <t>[
+            "$date": 1636982824139
+        },
+        "seat": "None"
+    },
     {
         "_id": {
-            "$oid": "61849d5f4367d925b16ff24c"
-        },
-        "city": "San Francisco",
-        "code": "SFO",
+            "$oid": "6192d0dbf5cb2f59a7dd4b6f"
+        },
+        "booking_history": "booked",
+        "booking_num": "#7B1P988X8KY7",
+        "customer_oid": {
+            "$oid": "618176b53dc26f93f1129a9d"
+        },
+        "flight_oid": "/flight/6192c60e35480dcd64335f6c",
+        "mileage_points_earned": 4,
         "modified_at": {
-            "$date": 1636055791184
-        },
-        "name": "San Francisco International Airport"
+            "$date": 1636982875220
+        },
+        "seat": "None"
     }
 ]</t>
   </si>
   <si>
-    <t>Admin required -- backend handled</t>
+    <r>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"flight_oid"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"6192ab07a2728d81e6aa6e11"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>}</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -496,44 +724,44 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
     <font>
       <sz val="8"/>
-      <color theme="1"/>
-      <name val="Calibri (Body)"/>
+      <color rgb="FF212121"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="8"/>
       <color rgb="FF6A8759"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF212121"/>
-      <name val="Helvetica"/>
+      <u/>
+      <sz val="8"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="6"/>
-      <color theme="1"/>
-      <name val="Calibri (Body)"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FFA31515"/>
-      <name val="Menlo"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -553,38 +781,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -897,136 +1124,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137CDCEF-55E1-8E4F-A1FE-9A17006F53F5}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="144" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="11"/>
   <cols>
-    <col min="1" max="2" width="7.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="7.83203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="36.5" style="4" customWidth="1"/>
-    <col min="8" max="8" width="22" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="2" width="7.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="36.5" style="8" customWidth="1"/>
+    <col min="8" max="8" width="22" style="7" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13">
-      <c r="B1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="3" t="s">
+    <row r="1" spans="1:9" ht="12">
+      <c r="B1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:9">
+      <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" ht="144">
+      <c r="C3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="156">
+      <c r="C4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" ht="156">
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="169">
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="48">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:9" ht="48">
+      <c r="A6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="96">
-      <c r="C7" s="3" t="s">
+    <row r="7" spans="1:9" ht="96">
+      <c r="C7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="9" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -1035,57 +1265,183 @@
       <c r="G7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="182">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:9" ht="144">
+      <c r="A9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3" t="b">
+      <c r="B9" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="9" t="s">
+    </row>
+    <row r="10" spans="1:9" ht="48">
+      <c r="C10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="11" t="s">
-        <v>28</v>
-      </c>
     </row>
-    <row r="10" spans="1:8" ht="409.6">
-      <c r="C10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="3" t="s">
+    <row r="11" spans="1:9" ht="405">
+      <c r="C11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>34</v>
+      <c r="E11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="306">
+      <c r="C13" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="144">
+      <c r="C14" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="48">
+      <c r="A16" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" ht="394">
+      <c r="C17" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" ht="192">
+      <c r="C19" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F14" r:id="rId1" xr:uid="{D61933BB-C4FA-004F-9390-6C905B683261}"/>
+    <hyperlink ref="F19" r:id="rId2" xr:uid="{1C6EF436-9EF7-804F-9B7A-BAAE16C4F292}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modfify flight price api | added logger | minor changes in f&b response
</commit_message>
<xml_diff>
--- a/API_documentation.xlsx
+++ b/API_documentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhitholar/college_work/cmpe202/team_project/team-project-team_techies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B37C742-5245-084F-B3D7-33D75F105959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2117CEE4-5946-AF4D-8F49-F323F8496DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10640" yWindow="-21100" windowWidth="28800" windowHeight="16240" xr2:uid="{AB8BB195-AD8F-664F-886C-5E9BDDAF898A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{AB8BB195-AD8F-664F-886C-5E9BDDAF898A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="73">
   <si>
     <t>Methid</t>
   </si>
@@ -424,76 +424,6 @@
   </si>
   <si>
     <t>http://127.0.0.1:5000/flight/6192ab07a2728d81e6aa6e11</t>
-  </si>
-  <si>
-    <t>{
-    "_id": {
-        "$oid": "6192ab07a2728d81e6aa6e11"
-    },
-    "aircraft": {
-        "$oid": "6184a9d1c2bf805a6ec5164a"
-    },
-    "arrival_airport": {
-        "$oid": "61849d3f4367d925b16ff24b"
-    },
-    "arrival_date": {
-        "$date": 1641427200000
-    },
-    "arrival_time": "11:00",
-    "departure_airport": {
-        "$oid": "61849d5f4367d925b16ff24c"
-    },
-    "departure_date": {
-        "$date": 1641427200000
-    },
-    "departure_time": "10:00",
-    "flight_num": "AA3455",
-    "flight_status": "scheduled",
-    "mileage_points": 4,
-    "modified_at": {
-        "$date": 1636973191119
-    },
-    "price": 40.0,
-    "remaining_seats": 60,
-    "seats": {
-        "aisle": 20,
-        "middle": 20,
-        "window": 20
-    }
-}</t>
-  </si>
-  <si>
-    <t>[
-    {
-        "_id": {
-            "$oid": "6192ab07a2728d81e6aa6e11"
-        },
-        "aircraft": "/aircraft/6184a9d1c2bf805a6ec5164a",
-        "arrival_airport": "/airport/61849d3f4367d925b16ff24b",
-        "arrival_date": {
-            "$date": 1641427200000
-        },
-        "arrival_time": "11:00",
-        "departure_airport": "/airport/61849d5f4367d925b16ff24c",
-        "departure_date": {
-            "$date": 1641427200000
-        },
-        "departure_time": "10:00",
-        "flight_num": "AA3455",
-        "flight_status": "scheduled",
-        "mileage_points": 4,
-        "modified_at": {
-            "$date": 1636973191119
-        },
-        "price": 40.0,
-        "remaining_seats": 60,
-        "seats": {
-            "aisle": 20,
-            "middle": 20,
-            "window": 20
-        }
-    }
-]</t>
   </si>
   <si>
     <t>Aircraft</t>
@@ -598,21 +528,126 @@
     <t>http://127.0.0.1:5000/booking/6192d0a8f5cb2f59a7dd4b6e</t>
   </si>
   <si>
+    <r>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"flight_oid"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"6192ab07a2728d81e6aa6e11"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>}</t>
+    </r>
+  </si>
+  <si>
+    <t>[
+    {
+        "_id": {
+            "$oid": "6192c60e35480dcd64335f6c"
+        },
+        "aircraft": {
+            "$oid": "6184a9d1c2bf805a6ec5164a"
+        },
+        "aircraft_details": "/aircraft/6184a9d1c2bf805a6ec5164a",
+        "arrival_airport": {
+            "$oid": "61849d5f4367d925b16ff24c"
+        },
+        "arrival_airport_details": "/airport/61849d5f4367d925b16ff24c",
+        "arrival_date": {
+            "$date": 1641427200000
+        },
+        "arrival_time": "11:00",
+        "departure_airport": {
+            "$oid": "61849d3f4367d925b16ff24b"
+        },
+        "departure_airport_details": "/airport/61849d3f4367d925b16ff24b",
+        "departure_date": {
+            "$date": 1641427200000
+        },
+        "departure_time": "10:00",
+        "flight_num": "AA1234",
+        "flight_status": "scheduled",
+        "mileage_points": 4,
+        "modified_at": {
+            "$date": 1636983180696
+        },
+        "price": 40.0,
+        "remaining_seats": 54,
+        "seats": {
+            "aisle": 20,
+            "middle": 20,
+            "window": 20
+        }
+    }
+]</t>
+  </si>
+  <si>
     <t>{
     "_id": {
-        "$oid": "6192d0a8f5cb2f59a7dd4b6e"
+        "$oid": "6192c60e35480dcd64335f6c"
     },
-    "booking_history": "booked",
-    "booking_num": "#940QL3FTF99N",
-    "customer_oid": {
-        "$oid": "618176b53dc26f93f1129a9d"
+    "aircraft": {
+        "$oid": "6184a9d1c2bf805a6ec5164a"
     },
-    "flight_oid": "/flight/6192c74866cb83011fbe931a",
-    "mileage_points_earned": 4,
+    "aircraft_details": "/aircraft/6184a9d1c2bf805a6ec5164a",
+    "arrival_airport": {
+        "$oid": "61849d5f4367d925b16ff24c"
+    },
+    "arrival_airport_details": "/airport/61849d5f4367d925b16ff24c",
+    "arrival_date": {
+        "$date": 1641427200000
+    },
+    "arrival_time": "11:00",
+    "departure_airport": {
+        "$oid": "61849d3f4367d925b16ff24b"
+    },
+    "departure_airport_details": "/airport/61849d3f4367d925b16ff24b",
+    "departure_date": {
+        "$date": 1641427200000
+    },
+    "departure_time": "10:00",
+    "flight_num": "AA1234",
+    "flight_status": "scheduled",
+    "mileage_points": 4,
     "modified_at": {
-        "$date": 1636982824139
+        "$date": 1636983180696
     },
-    "seat": "None"
+    "price": 40.0,
+    "remaining_seats": 54,
+    "seats": {
+        "aisle": 20,
+        "middle": 20,
+        "window": 20
+    }
 }</t>
   </si>
   <si>
@@ -626,7 +661,10 @@
         "customer_oid": {
             "$oid": "618176b53dc26f93f1129a9d"
         },
-        "flight_oid": "/flight/6192c74866cb83011fbe931a",
+        "flight_details": "/flight/6192c74866cb83011fbe931a",
+        "flight_oid": {
+            "$oid": "6192c74866cb83011fbe931a"
+        },
         "mileage_points_earned": 4,
         "modified_at": {
             "$date": 1636982824139
@@ -642,7 +680,10 @@
         "customer_oid": {
             "$oid": "618176b53dc26f93f1129a9d"
         },
-        "flight_oid": "/flight/6192c60e35480dcd64335f6c",
+        "flight_details": "/flight/6192c60e35480dcd64335f6c",
+        "flight_oid": {
+            "$oid": "6192c60e35480dcd64335f6c"
+        },
         "mileage_points_earned": 4,
         "modified_at": {
             "$date": 1636982875220
@@ -652,45 +693,46 @@
 ]</t>
   </si>
   <si>
-    <r>
-      <t>{</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>"flight_oid"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF0451A5"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>"6192ab07a2728d81e6aa6e11"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>}</t>
-    </r>
+    <t xml:space="preserve"> {
+        "_id": {
+            "$oid": "6192d0a8f5cb2f59a7dd4b6e"
+        },
+        "booking_history": "booked",
+        "booking_num": "#940QL3FTF99N",
+        "customer_oid": {
+            "$oid": "618176b53dc26f93f1129a9d"
+        },
+        "flight_details": "/flight/6192c74866cb83011fbe931a",
+        "flight_oid": {
+            "$oid": "6192c74866cb83011fbe931a"
+        },
+        "mileage_points_earned": 4,
+        "modified_at": {
+            "$date": 1636982824139
+        },
+        "seat": "None"
+    },</t>
+  </si>
+  <si>
+    <t>Update Price</t>
+  </si>
+  <si>
+    <t>Put</t>
+  </si>
+  <si>
+    <t>{   "flight_id" : "6192c60e35480dcd64335f6c",
+    "price" : 50
+}</t>
+  </si>
+  <si>
+    <t>{
+    "message": "Flight update successful"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "message": "No such flight exists"
+}</t>
   </si>
 </sst>
 </file>
@@ -785,7 +827,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -800,7 +842,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1124,119 +1165,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137CDCEF-55E1-8E4F-A1FE-9A17006F53F5}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="144" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="144" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11"/>
   <cols>
-    <col min="1" max="2" width="7.83203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="7.83203125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="36.5" style="8" customWidth="1"/>
-    <col min="8" max="8" width="22" style="7" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="7"/>
+    <col min="1" max="2" width="7.83203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="36.5" style="7" customWidth="1"/>
+    <col min="8" max="8" width="22" style="6" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="12">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="7" t="b">
+      <c r="B2" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="7"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:9" ht="144">
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="156">
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="48">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -1250,13 +1291,13 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="96">
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -1270,22 +1311,22 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="144">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="7" t="b">
+      <c r="B9" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="7" t="s">
         <v>38</v>
       </c>
       <c r="G9" s="4" t="s">
@@ -1295,146 +1336,169 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="48">
-      <c r="C10" s="7" t="s">
+    <row r="10" spans="1:9" ht="409.6">
+      <c r="C10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10" s="7" t="s">
+      <c r="G10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="405">
-      <c r="C11" s="7" t="s">
+    <row r="11" spans="1:9" ht="409.6">
+      <c r="C11" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>41</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>43</v>
+      <c r="G11" s="7" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="7" t="b">
+      <c r="A12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>51</v>
+      <c r="C12" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="306">
-      <c r="C13" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="C13" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>46</v>
+      <c r="E13" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="144">
-      <c r="C14" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="7" t="s">
+      <c r="C14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="48">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="F16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G16" s="8" t="s">
+      <c r="I16" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="409.6">
+      <c r="C17" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="H16" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="I16" s="8" t="s">
+      <c r="D17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" ht="394">
-      <c r="C17" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="H17" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="3:8" ht="192">
-      <c r="C19" s="7" t="s">
+    <row r="19" spans="1:8" ht="228">
+      <c r="C19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>65</v>
+      <c r="G19" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="48">
+      <c r="A21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
purchase seat api | get_user_details API | removed HATEOs and added data in response
</commit_message>
<xml_diff>
--- a/API_documentation.xlsx
+++ b/API_documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhitholar/college_work/cmpe202/team_project/team-project-team_techies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2117CEE4-5946-AF4D-8F49-F323F8496DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806912B4-DE20-9C46-A288-F2DB759E897F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{AB8BB195-AD8F-664F-886C-5E9BDDAF898A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{AB8BB195-AD8F-664F-886C-5E9BDDAF898A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="85">
   <si>
     <t>Methid</t>
   </si>
@@ -81,9 +81,6 @@
     <t>User login</t>
   </si>
   <si>
-    <t>/user-login</t>
-  </si>
-  <si>
     <t>Flight</t>
   </si>
   <si>
@@ -252,16 +249,6 @@
   </si>
   <si>
     <t>"User - john1@gmail.com registered successfully"</t>
-  </si>
-  <si>
-    <t>{
-    "message": "User - nidhi@gmail.com login successfully",
-    "user": {
-        "email": "nidhi@gmail.com",
-        "first_name": "nidhi",
-        "last_name": "tholar"
-    }
-}</t>
   </si>
   <si>
     <t>{
@@ -504,11 +491,6 @@
   </si>
   <si>
     <t>{
-    "message": "Booking successful"
-}</t>
-  </si>
-  <si>
-    <t>{
     "message": "Flight is full"
 }</t>
   </si>
@@ -528,45 +510,80 @@
     <t>http://127.0.0.1:5000/booking/6192d0a8f5cb2f59a7dd4b6e</t>
   </si>
   <si>
-    <r>
-      <t>{</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>"flight_oid"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF0451A5"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>"6192ab07a2728d81e6aa6e11"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>}</t>
-    </r>
+    <t>[
+    {
+        "_id": {
+            "$oid": "6192d0a8f5cb2f59a7dd4b6e"
+        },
+        "booking_history": "booked",
+        "booking_num": "#940QL3FTF99N",
+        "customer_oid": {
+            "$oid": "618176b53dc26f93f1129a9d"
+        },
+        "flight_details": "/flight/6192c74866cb83011fbe931a",
+        "flight_oid": {
+            "$oid": "6192c74866cb83011fbe931a"
+        },
+        "mileage_points_earned": 4,
+        "modified_at": {
+            "$date": 1636982824139
+        },
+        "seat": "None"
+    },
+    {
+        "_id": {
+            "$oid": "6192d0dbf5cb2f59a7dd4b6f"
+        },
+        "booking_history": "booked",
+        "booking_num": "#7B1P988X8KY7",
+        "customer_oid": {
+            "$oid": "618176b53dc26f93f1129a9d"
+        },
+        "flight_details": "/flight/6192c60e35480dcd64335f6c",
+        "flight_oid": {
+            "$oid": "6192c60e35480dcd64335f6c"
+        },
+        "mileage_points_earned": 4,
+        "modified_at": {
+            "$date": 1636982875220
+        },
+        "seat": "None"
+    }
+]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {
+        "_id": {
+            "$oid": "6192d0a8f5cb2f59a7dd4b6e"
+        },
+        "booking_history": "booked",
+        "booking_num": "#940QL3FTF99N",
+        "customer_oid": {
+            "$oid": "618176b53dc26f93f1129a9d"
+        },
+        "flight_details": "/flight/6192c74866cb83011fbe931a",
+        "flight_oid": {
+            "$oid": "6192c74866cb83011fbe931a"
+        },
+        "mileage_points_earned": 4,
+        "modified_at": {
+            "$date": 1636982824139
+        },
+        "seat": "None"
+    },</t>
+  </si>
+  <si>
+    <t>Put</t>
+  </si>
+  <si>
+    <t>{
+    "message": "Flight update successful"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "message": "No such flight exists"
+}</t>
   </si>
   <si>
     <t>[
@@ -575,21 +592,25 @@
             "$oid": "6192c60e35480dcd64335f6c"
         },
         "aircraft": {
-            "$oid": "6184a9d1c2bf805a6ec5164a"
-        },
-        "aircraft_details": "/aircraft/6184a9d1c2bf805a6ec5164a",
+            "$oid": "6184a9d1c2bf805a6ec5164a",
+            "name": "Boeing 737"
+        },
         "arrival_airport": {
-            "$oid": "61849d5f4367d925b16ff24c"
-        },
-        "arrival_airport_details": "/airport/61849d5f4367d925b16ff24c",
+            "$oid": "61849d5f4367d925b16ff24c",
+            "city": "San Francisco",
+            "code": "SFO",
+            "name": "San Francisco International Airport"
+        },
         "arrival_date": {
             "$date": 1641427200000
         },
         "arrival_time": "11:00",
         "departure_airport": {
-            "$oid": "61849d3f4367d925b16ff24b"
-        },
-        "departure_airport_details": "/airport/61849d3f4367d925b16ff24b",
+            "$oid": "61849d3f4367d925b16ff24b",
+            "city": "San Jose",
+            "code": "SJC",
+            "name": "San Jose International Airport"
+        },
         "departure_date": {
             "$date": 1641427200000
         },
@@ -598,9 +619,9 @@
         "flight_status": "scheduled",
         "mileage_points": 4,
         "modified_at": {
-            "$date": 1636983180696
-        },
-        "price": 40.0,
+            "$date": 1637159368425
+        },
+        "price": 50.0,
         "remaining_seats": 54,
         "seats": {
             "aisle": 20,
@@ -613,125 +634,182 @@
   <si>
     <t>{
     "_id": {
-        "$oid": "6192c60e35480dcd64335f6c"
+        "$oid": "6192c74866cb83011fbe931a"
     },
     "aircraft": {
-        "$oid": "6184a9d1c2bf805a6ec5164a"
+        "$oid": "6184a9d1c2bf805a6ec5164a",
+        "name": "Boeing 737"
     },
-    "aircraft_details": "/aircraft/6184a9d1c2bf805a6ec5164a",
     "arrival_airport": {
-        "$oid": "61849d5f4367d925b16ff24c"
+        "$oid": "61849d3f4367d925b16ff24b",
+        "city": "San Jose",
+        "code": "SJC",
+        "name": "San Jose International Airport"
     },
-    "arrival_airport_details": "/airport/61849d5f4367d925b16ff24c",
     "arrival_date": {
-        "$date": 1641427200000
+        "$date": 1641686400000
     },
-    "arrival_time": "11:00",
+    "arrival_time": "21:00",
     "departure_airport": {
-        "$oid": "61849d3f4367d925b16ff24b"
+        "$oid": "61849d5f4367d925b16ff24c",
+        "city": "San Francisco",
+        "code": "SFO",
+        "name": "San Francisco International Airport"
     },
-    "departure_airport_details": "/airport/61849d3f4367d925b16ff24b",
     "departure_date": {
-        "$date": 1641427200000
+        "$date": 1641686400000
     },
-    "departure_time": "10:00",
-    "flight_num": "AA1234",
+    "departure_time": "20:00",
+    "flight_num": "AA7891",
     "flight_status": "scheduled",
     "mileage_points": 4,
     "modified_at": {
-        "$date": 1636983180696
+        "$date": 1636982824269
     },
     "price": 40.0,
-    "remaining_seats": 54,
+    "remaining_seats": 0,
     "seats": {
-        "aisle": 20,
-        "middle": 20,
-        "window": 20
+        "aisle": 1,
+        "middle": 0,
+        "window": 1
     }
 }</t>
   </si>
   <si>
-    <t>[
-    {
+    <t>ADMIN APIS:</t>
+  </si>
+  <si>
+    <t>Get all flights</t>
+  </si>
+  <si>
+    <t>Get</t>
+  </si>
+  <si>
+    <t>/flight/&lt;id&gt;</t>
+  </si>
+  <si>
+    <t>Update Flight ( price, status)</t>
+  </si>
+  <si>
+    <t>{   "flight_id" : "6192c60e35480dcd64335f6c",
+    "price" : 100,
+    "flight_status" : "canceled"
+} Include the fields if it needs to be modified
+//  choices for flight_status=['scheduled', 'canceled']</t>
+  </si>
+  <si>
+    <t>{"flight_oid": "6192cf0795636ba8b9bf824a",
+"traveler_details": {"name":"xyz"},
+"payment" :{ "reward_points_used" : 20,
+  "cash": 50}
+}</t>
+  </si>
+  <si>
+    <t>{
+    "booking": {
         "_id": {
-            "$oid": "6192d0a8f5cb2f59a7dd4b6e"
-        },
+            "$oid": "6199f9a9c0c799c3792a951e"
+        },
+        "booked_price": 40,
         "booking_history": "booked",
-        "booking_num": "#940QL3FTF99N",
+        "booking_num": "#0RLJ8WEJSHF7",
         "customer_oid": {
             "$oid": "618176b53dc26f93f1129a9d"
         },
-        "flight_details": "/flight/6192c74866cb83011fbe931a",
+        "flight_oid": {
+            "$oid": "6192cf0795636ba8b9bf824a"
+        },
+        "flight_status": "scheduled",
+        "mileage_points_earned": 4.0,
+        "modified_at": {
+            "$date": 1637452073138
+        },
+        "payment": {
+            "cash": 50,
+            "reward_points_used": 20
+        },
+        "seat": "None",
+        "traveller_details": {
+            "name": "xyz"
+        }
+    },
+    "message": "Booking successful"
+}</t>
+  </si>
+  <si>
+    <t>/user</t>
+  </si>
+  <si>
+    <t>{
+    "message": "User - nidhi@gmail.com login successfully",
+    "user": {
+        "first_name": "nidhi",
+        "user_type": "admin"
+    }
+}</t>
+  </si>
+  <si>
+    <t>Get user details</t>
+  </si>
+  <si>
+    <t>{
+    "email": "nidhi@gmail.com",
+    "first_name": "nidhi",
+    "last_name": "tholar",
+    "mileage_points": 10.0,
+    "user_type": "admin"
+}</t>
+  </si>
+  <si>
+    <t>Purchase Seat</t>
+  </si>
+  <si>
+    <t>/booking/purchase_seat</t>
+  </si>
+  <si>
+    <t>{
+    "booking": {
+        "_id": {
+            "$oid": "619a0f85e05c0e2541955824"
+        },
+        "booked_price": 40,
+        "booking_history": "booked",
+        "booking_num": "#S1KQVXANVDCD",
+        "customer_oid": {
+            "$oid": "618176b53dc26f93f1129a9d"
+        },
         "flight_oid": {
             "$oid": "6192c74866cb83011fbe931a"
         },
-        "mileage_points_earned": 4,
+        "flight_status": "scheduled",
+        "mileage_points_earned": 4.0,
         "modified_at": {
-            "$date": 1636982824139
-        },
-        "seat": "None"
+            "$date": 1637457703341
+        },
+        "payment": {
+            "cash": 50,
+            "reward_points_used": 20
+        },
+        "seat": "window",
+        "traveller_details": {
+            "name": "xyz"
+        }
     },
-    {
-        "_id": {
-            "$oid": "6192d0dbf5cb2f59a7dd4b6f"
-        },
-        "booking_history": "booked",
-        "booking_num": "#7B1P988X8KY7",
-        "customer_oid": {
-            "$oid": "618176b53dc26f93f1129a9d"
-        },
-        "flight_details": "/flight/6192c60e35480dcd64335f6c",
-        "flight_oid": {
-            "$oid": "6192c60e35480dcd64335f6c"
-        },
-        "mileage_points_earned": 4,
-        "modified_at": {
-            "$date": 1636982875220
-        },
-        "seat": "None"
-    }
-]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> {
-        "_id": {
-            "$oid": "6192d0a8f5cb2f59a7dd4b6e"
-        },
-        "booking_history": "booked",
-        "booking_num": "#940QL3FTF99N",
-        "customer_oid": {
-            "$oid": "618176b53dc26f93f1129a9d"
-        },
-        "flight_details": "/flight/6192c74866cb83011fbe931a",
-        "flight_oid": {
-            "$oid": "6192c74866cb83011fbe931a"
-        },
-        "mileage_points_earned": 4,
-        "modified_at": {
-            "$date": 1636982824139
-        },
-        "seat": "None"
-    },</t>
-  </si>
-  <si>
-    <t>Update Price</t>
-  </si>
-  <si>
-    <t>Put</t>
-  </si>
-  <si>
-    <t>{   "flight_id" : "6192c60e35480dcd64335f6c",
-    "price" : 50
+    "message": "Seat Purchase successful!"
 }</t>
   </si>
   <si>
+    <t>{"booking_id" :"619a0f85e05c0e2541955824",
+"seat":"window"}</t>
+  </si>
+  <si>
     <t>{
-    "message": "Flight update successful"
+    "message": "You have already booked a seat for this flight!!"
 }</t>
   </si>
   <si>
     <t>{
-    "message": "No such flight exists"
+    "message": "All window seats are taken"
 }</t>
   </si>
 </sst>
@@ -739,7 +817,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -805,6 +883,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFA31515"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -827,7 +917,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -848,6 +938,10 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1165,10 +1259,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137CDCEF-55E1-8E4F-A1FE-9A17006F53F5}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="144" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="144" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11"/>
@@ -1176,7 +1270,7 @@
     <col min="1" max="2" width="7.83203125" style="6" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="7.83203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" style="6" customWidth="1"/>
     <col min="6" max="6" width="25.33203125" style="7" customWidth="1"/>
     <col min="7" max="7" width="36.5" style="7" customWidth="1"/>
     <col min="8" max="8" width="22" style="6" customWidth="1"/>
@@ -1185,7 +1279,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="12">
       <c r="B1" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>2</v>
@@ -1197,13 +1291,13 @@
         <v>1</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1223,7 +1317,7 @@
         <v>5</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G2" s="6"/>
     </row>
@@ -1238,13 +1332,13 @@
         <v>5</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="156">
@@ -1258,13 +1352,13 @@
         <v>9</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="48">
@@ -1281,16 +1375,16 @@
         <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="96">
+    </row>
+    <row r="7" spans="1:9" ht="84">
       <c r="C7" s="6" t="s">
         <v>14</v>
       </c>
@@ -1298,207 +1392,275 @@
         <v>4</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="84">
+      <c r="C8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="144">
       <c r="A9" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="6" t="b">
         <v>1</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="409.6">
       <c r="C10" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="409.6">
       <c r="C11" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B12" s="6" t="b">
         <v>1</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="306">
       <c r="C13" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="144">
       <c r="C14" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="48">
+    </row>
+    <row r="16" spans="1:9" ht="350">
       <c r="A16" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E16" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I16" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16" s="7" t="s">
+    </row>
+    <row r="17" spans="1:9" ht="409.6">
+      <c r="C17" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="409.6">
-      <c r="C17" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="228">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="228">
       <c r="C19" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E19" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F19" s="9" t="s">
+    </row>
+    <row r="21" spans="1:9" ht="350">
+      <c r="A21" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="12">
+      <c r="F22" s="10"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="12">
+      <c r="A26" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="84">
+      <c r="A28" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="48">
-      <c r="A21" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="7" t="s">
+      <c r="E28" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G21" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H21" s="7" t="s">
+      <c r="F28" s="7" t="s">
         <v>72</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cancel and change booking | purchase seat
</commit_message>
<xml_diff>
--- a/API_documentation.xlsx
+++ b/API_documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhitholar/college_work/cmpe202/team_project/team-project-team_techies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806912B4-DE20-9C46-A288-F2DB759E897F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67782F87-796F-7C46-8538-E78C5D45BB37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{AB8BB195-AD8F-664F-886C-5E9BDDAF898A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{AB8BB195-AD8F-664F-886C-5E9BDDAF898A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="96">
   <si>
     <t>Methid</t>
   </si>
@@ -812,12 +812,59 @@
     "message": "All window seats are taken"
 }</t>
   </si>
+  <si>
+    <t>Change/Cancel</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:5000/booking/619ac7ef63b736cef9773d68</t>
+  </si>
+  <si>
+    <t>{
+    "message": "Booking #M1ZE6H5CT9PB canceled successfully"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "message": "Booking not found"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "message": "Booking is already canceled"
+}</t>
+  </si>
+  <si>
+    <t>Change</t>
+  </si>
+  <si>
+    <t>{
+    "message": "You can change the Booking only once!!"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "booking_id":"619ade645bf1fa1382a63771",
+    "flight_oid": "619ac7a563b736cef9773d67",
+"traveler_details": {"name":"xyz"},
+"payment" :{ "reward_points_used" : 20,
+  "cash": 50}
+}</t>
+  </si>
+  <si>
+    <t>Booking  changed successfully</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -895,6 +942,12 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212121"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -917,7 +970,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -942,6 +995,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1259,10 +1315,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137CDCEF-55E1-8E4F-A1FE-9A17006F53F5}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="144" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="144" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11"/>
@@ -1663,6 +1719,57 @@
         <v>64</v>
       </c>
     </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="61">
+      <c r="A32" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" ht="108">
+      <c r="C34" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F14" r:id="rId1" xr:uid="{D61933BB-C4FA-004F-9390-6C905B683261}"/>

</xml_diff>

<commit_message>
get setas API | modified other APIs for seat num
</commit_message>
<xml_diff>
--- a/API_documentation.xlsx
+++ b/API_documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhitholar/college_work/cmpe202/team_project/team-project-team_techies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C87E9A-2E95-3740-A2F8-FACDD95D554D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6116F258-CD7E-D54F-ACB9-DCA91E30E38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{AB8BB195-AD8F-664F-886C-5E9BDDAF898A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="100">
   <si>
     <t>Methid</t>
   </si>
@@ -799,10 +799,6 @@
 }</t>
   </si>
   <si>
-    <t>{"booking_id" :"619a0f85e05c0e2541955824",
-"seat":"window"}</t>
-  </si>
-  <si>
     <t>{
     "message": "You have already booked a seat for this flight!!"
 }</t>
@@ -858,6 +854,45 @@
   </si>
   <si>
     <t>Booking  changed successfully</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:5000/booking/purchase_seat/619af748753af0eea133e3e2</t>
+  </si>
+  <si>
+    <t>Get seats</t>
+  </si>
+  <si>
+    <t>/booking/purchase_seat/&lt;id&gt;</t>
+  </si>
+  <si>
+    <t>{
+    "num_of_seats": {
+        "aisle": 20,
+        "middle": 20,
+        "window": 19
+    },
+    "price": {
+        "aisle": 3,
+        "middle": 0,
+        "window": 5
+    },
+    "seat_num": {
+        "aisle": [
+            "1A"
+        ],
+        "middle": [
+            "1B"
+        ],
+        "window": [
+            "1C"
+        ]
+    }
+}</t>
+  </si>
+  <si>
+    <t>{"booking_id" :"61a276afea9044c96dd4c200",
+"seat_type":"window",
+"seat_num": "2C"}</t>
   </si>
 </sst>
 </file>
@@ -937,16 +972,16 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FFA31515"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF212121"/>
       <name val="Helvetica"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -970,7 +1005,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -993,13 +1028,16 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1317,8 +1355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137CDCEF-55E1-8E4F-A1FE-9A17006F53F5}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="144" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="144" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11"/>
@@ -1658,21 +1696,35 @@
       <c r="E21" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F21" s="11" t="s">
-        <v>82</v>
+      <c r="F21" s="10" t="s">
+        <v>99</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>81</v>
       </c>
       <c r="H21" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I21" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="I21" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="12">
-      <c r="F22" s="10"/>
+    </row>
+    <row r="22" spans="1:9" ht="274">
+      <c r="C22" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="6" t="s">
@@ -1721,7 +1773,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="61">
@@ -1729,30 +1781,30 @@
         <v>50</v>
       </c>
       <c r="C32" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>87</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>58</v>
       </c>
       <c r="F32" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G32" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G32" s="7" t="s">
+      <c r="H32" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="H32" s="7" t="s">
+      <c r="I32" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="34" spans="3:8" ht="108">
       <c r="C34" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>62</v>
@@ -1761,19 +1813,20 @@
         <v>52</v>
       </c>
       <c r="F34" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G34" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G34" s="7" t="s">
-        <v>95</v>
-      </c>
       <c r="H34" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F14" r:id="rId1" xr:uid="{D61933BB-C4FA-004F-9390-6C905B683261}"/>
     <hyperlink ref="F19" r:id="rId2" xr:uid="{1C6EF436-9EF7-804F-9B7A-BAAE16C4F292}"/>
+    <hyperlink ref="F32" r:id="rId3" xr:uid="{923A6D88-DBBA-E946-B884-E1A396DDAB1E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed booking API to get flight data in response instead of HATEOS
</commit_message>
<xml_diff>
--- a/API_documentation.xlsx
+++ b/API_documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhitholar/college_work/cmpe202/team_project/team-project-team_techies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6116F258-CD7E-D54F-ACB9-DCA91E30E38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5007FA4D-A61C-AF4F-AED0-5E19143966EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{AB8BB195-AD8F-664F-886C-5E9BDDAF898A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="99">
   <si>
     <t>Methid</t>
   </si>
@@ -508,48 +508,6 @@
   </si>
   <si>
     <t>http://127.0.0.1:5000/booking/6192d0a8f5cb2f59a7dd4b6e</t>
-  </si>
-  <si>
-    <t>[
-    {
-        "_id": {
-            "$oid": "6192d0a8f5cb2f59a7dd4b6e"
-        },
-        "booking_history": "booked",
-        "booking_num": "#940QL3FTF99N",
-        "customer_oid": {
-            "$oid": "618176b53dc26f93f1129a9d"
-        },
-        "flight_details": "/flight/6192c74866cb83011fbe931a",
-        "flight_oid": {
-            "$oid": "6192c74866cb83011fbe931a"
-        },
-        "mileage_points_earned": 4,
-        "modified_at": {
-            "$date": 1636982824139
-        },
-        "seat": "None"
-    },
-    {
-        "_id": {
-            "$oid": "6192d0dbf5cb2f59a7dd4b6f"
-        },
-        "booking_history": "booked",
-        "booking_num": "#7B1P988X8KY7",
-        "customer_oid": {
-            "$oid": "618176b53dc26f93f1129a9d"
-        },
-        "flight_details": "/flight/6192c60e35480dcd64335f6c",
-        "flight_oid": {
-            "$oid": "6192c60e35480dcd64335f6c"
-        },
-        "mileage_points_earned": 4,
-        "modified_at": {
-            "$date": 1636982875220
-        },
-        "seat": "None"
-    }
-]</t>
   </si>
   <si>
     <t xml:space="preserve"> {
@@ -685,9 +643,6 @@
     <t>Get</t>
   </si>
   <si>
-    <t>/flight/&lt;id&gt;</t>
-  </si>
-  <si>
     <t>Update Flight ( price, status)</t>
   </si>
   <si>
@@ -893,6 +848,91 @@
     <t>{"booking_id" :"61a276afea9044c96dd4c200",
 "seat_type":"window",
 "seat_num": "2C"}</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "_id": {
+            "$oid": "61a276afea9044c96dd4c200"
+        },
+        "booked_price": 40,
+        "booking_history": "booked",
+        "booking_num": "#UWJH25G7UTCE",
+        "customer_oid": {
+            "$oid": "618176b53dc26f93f1129a9d"
+        },
+        "flight_oid": {
+            "_id": {
+                "$oid": "61a26d7d500dc3da968da8f1"
+            },
+            "aircraft": {
+                "$oid": "6184a9d1c2bf805a6ec5164a",
+                "name": "Boeing 737"
+            },
+            "arrival_airport": {
+                "$oid": "61849d3f4367d925b16ff24b",
+                "city": "San Jose",
+                "code": "SJC",
+                "name": "San Jose International Airport"
+            },
+            "arrival_date": {
+                "$date": 1641686400000
+            },
+            "arrival_time": "08:00",
+            "departure_airport": {
+                "$oid": "61849d5f4367d925b16ff24c",
+                "city": "San Francisco",
+                "code": "SFO",
+                "name": "San Francisco International Airport"
+            },
+            "departure_date": {
+                "$date": 1641686400000
+            },
+            "departure_time": "07:00",
+            "flight_num": "AA3457",
+            "flight_status": "scheduled",
+            "modified_at": {
+                "$date": 1638019405576
+            },
+            "price": 40.0,
+            "remaining_seats": 59,
+            "seat_chart": {
+                "aisle": [
+                    "1A"
+                ],
+                "middle": [
+                    "1B"
+                ],
+                "window": []
+            },
+            "seat_price": {
+                "aisle": 3,
+                "middle": 0,
+                "window": 5
+            },
+            "seats": {
+                "aisle": 20,
+                "middle": 20,
+                "window": 16
+            }
+        },
+        "flight_status": "scheduled",
+        "mileage_points_earned": 6.0,
+        "modified_at": {
+            "$date": 1638019405581
+        },
+        "payment": {
+            "cash": 30,
+            "reward_points_used": 10
+        },
+        "seat_num": "1C",
+        "seat_price": 5,
+        "seat_type": "window",
+        "traveller_details": {
+            "name": "xyz"
+        }
+    }
+]</t>
   </si>
 </sst>
 </file>
@@ -1355,8 +1395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137CDCEF-55E1-8E4F-A1FE-9A17006F53F5}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="144" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="144" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11"/>
@@ -1486,13 +1526,13 @@
         <v>4</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>23</v>
@@ -1500,19 +1540,19 @@
     </row>
     <row r="8" spans="1:9" ht="84">
       <c r="C8" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>31</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="144">
@@ -1555,7 +1595,7 @@
         <v>28</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>29</v>
@@ -1575,7 +1615,7 @@
         <v>40</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1634,10 +1674,10 @@
         <v>52</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>53</v>
@@ -1660,7 +1700,7 @@
         <v>56</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="H17" s="6" t="s">
         <v>29</v>
@@ -1680,55 +1720,55 @@
         <v>59</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="350">
       <c r="A21" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E21" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H21" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F21" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="G21" s="7" t="s">
+      <c r="I21" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="274">
       <c r="C22" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="12">
@@ -1736,10 +1776,10 @@
         <v>15</v>
       </c>
       <c r="C26" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>17</v>
@@ -1753,27 +1793,27 @@
         <v>15</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D28" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G28" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="G28" s="7" t="s">
+      <c r="H28" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="61">
@@ -1781,45 +1821,45 @@
         <v>50</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>58</v>
       </c>
       <c r="F32" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H32" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="G32" s="7" t="s">
+      <c r="I32" s="7" t="s">
         <v>88</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="34" spans="3:8" ht="108">
       <c r="C34" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>52</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes for json error
</commit_message>
<xml_diff>
--- a/API_documentation.xlsx
+++ b/API_documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhitholar/college_work/cmpe202/team_project/team-project-team_techies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56652460-94D5-7945-BB92-2688E482C5C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE600A70-371F-B34D-ABC9-2A39106715F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{AB8BB195-AD8F-664F-886C-5E9BDDAF898A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{AB8BB195-AD8F-664F-886C-5E9BDDAF898A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="105">
   <si>
     <t>Methid</t>
   </si>
@@ -1035,6 +1035,102 @@
         }
     }
 ]</t>
+  </si>
+  <si>
+    <t>new Response</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "city": "San Jose",
+        "code": "SJC",
+        "id": "61849d3f4367d925b16ff24b",
+        "name": "San Jose International Airport"
+    },
+    {
+        "city": "San Francisco",
+        "code": "SFO",
+        "id": "61849d5f4367d925b16ff24c",
+        "name": "San Francisco International Airport"
+    }]</t>
+  </si>
+  <si>
+    <t>{
+    "city": "San Jose",
+    "code": "SJC",
+    "id": "61849d3f4367d925b16ff24b",
+    "name": "San Jose International Airport"
+}</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "id": "61a5aac8b657dbd44f933bb9",
+        "name": "Airbus A320",
+        "seat_chart": {
+            "aisle": [
+                "1A"
+            ],
+            "middle": [
+                "1B"
+            ],
+            "window": [
+                "1C"
+            ]
+        },
+        "total_seats": 90
+    },
+    {
+        "id": "61a5ab60b657dbd44f933bba",
+        "name": "Boeing 747",
+        "seat_chart": {
+            "aisle": [
+                "1A"
+            ],
+            "middle": [
+                "1B"
+            ],
+            "window": [
+                "1C"
+            ]
+        },
+        "total_seats": 90
+    },
+    {
+        "id": "61a5abf6b657dbd44f933bbb",
+        "name": "Airbus A520",
+        "seat_chart": {
+            "aisle": [
+                "1A"
+            ],
+            "middle": [
+                "1B"
+            ],
+            "window": [
+                "1C"
+            ]
+        },
+        "total_seats": 90
+    }
+]</t>
+  </si>
+  <si>
+    <t>{
+    "id": "61a5aac8b657dbd44f933bb9",
+    "name": "Airbus A320",
+    "seat_chart": {
+        "aisle": [
+            "1A"
+        ],
+        "middle": [
+            "1B"
+        ],
+        "window": [
+            "1C"
+        ]
+    },
+    "total_seats": 90
+}</t>
   </si>
 </sst>
 </file>
@@ -1497,8 +1593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137CDCEF-55E1-8E4F-A1FE-9A17006F53F5}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="144" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="144" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11"/>
@@ -1509,8 +1605,9 @@
     <col min="5" max="5" width="14.83203125" style="6" customWidth="1"/>
     <col min="6" max="6" width="25.33203125" style="7" customWidth="1"/>
     <col min="7" max="7" width="36.5" style="7" customWidth="1"/>
-    <col min="8" max="8" width="22" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="6"/>
+    <col min="8" max="8" width="11.1640625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="24.33203125" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="12">
@@ -1535,6 +1632,9 @@
       <c r="H1" s="6" t="s">
         <v>27</v>
       </c>
+      <c r="I1" s="6" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="6" t="s">
@@ -1557,7 +1657,7 @@
       </c>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="144">
+    <row r="3" spans="1:9" ht="295">
       <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1575,6 +1675,9 @@
       </c>
       <c r="H3" s="6" t="s">
         <v>29</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="156">
@@ -1596,6 +1699,9 @@
       <c r="H4" s="6" t="s">
         <v>29</v>
       </c>
+      <c r="I4" s="7" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="48">
       <c r="A6" s="6" t="s">
@@ -1731,7 +1837,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="306">
+    <row r="13" spans="1:9" ht="409.6">
       <c r="C13" s="6" t="s">
         <v>48</v>
       </c>
@@ -1744,8 +1850,11 @@
       <c r="G13" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="144">
+      <c r="I13" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="192">
       <c r="C14" s="6" t="s">
         <v>49</v>
       </c>
@@ -1760,6 +1869,9 @@
       </c>
       <c r="G14" s="7" t="s">
         <v>46</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="350">

</xml_diff>

<commit_message>
flight API changes for json error
</commit_message>
<xml_diff>
--- a/API_documentation.xlsx
+++ b/API_documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhitholar/college_work/cmpe202/team_project/team-project-team_techies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE600A70-371F-B34D-ABC9-2A39106715F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F58AD4-B93B-3E43-AAD9-455DF8068499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{AB8BB195-AD8F-664F-886C-5E9BDDAF898A}"/>
+    <workbookView xWindow="11640" yWindow="-20260" windowWidth="28800" windowHeight="18040" xr2:uid="{AB8BB195-AD8F-664F-886C-5E9BDDAF898A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="107">
   <si>
     <t>Methid</t>
   </si>
@@ -1130,6 +1130,108 @@
         ]
     },
     "total_seats": 90
+}</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "aircraft": {
+            "id": "61a5aac8b657dbd44f933bb9",
+            "name": "Airbus A320"
+        },
+        "arrival_airport": {
+            "city": "San Francisco",
+            "code": "SFO",
+            "id": "61849d5f4367d925b16ff24c",
+            "name": "San Francisco International Airport"
+        },
+        "arrival_date": "Sun, 09 Jan 2022 00:00:00 GMT",
+        "arrival_time": "08:00",
+        "departure_airport": {
+            "city": "San Jose",
+            "code": "SJC",
+            "id": "61849d3f4367d925b16ff24b",
+            "name": "San Jose International Airport"
+        },
+        "departure_date": "Sun, 09 Jan 2022 00:00:00 GMT",
+        "departure_time": "07:00",
+        "flight_num": "AA3457",
+        "flight_status": "scheduled",
+        "id": "61a5ae2a46401bf4c54c8c1e",
+        "price": "40.00",
+        "remaining_seats": 90,
+        "seat_chart": {
+            "aisle": [
+                "1A"
+            ],
+            "middle": [
+                "1B"
+            ],
+            "window": [
+                "1C"
+            ]
+        },
+        "seat_price": {
+            "aisle": 3,
+            "middle": 0,
+            "window": 5
+        },
+        "seats": {
+            "aisle": 30,
+            "middle": 30,
+            "window": 30
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>{
+    "aircraft": {
+        "id": "61a5aac8b657dbd44f933bb9",
+        "name": "Airbus A320"
+    },
+    "arrival_airport": {
+        "city": "San Francisco",
+        "code": "SFO",
+        "id": "61849d5f4367d925b16ff24c",
+        "name": "San Francisco International Airport"
+    },
+    "arrival_date": "Sun, 09 Jan 2022 00:00:00 GMT",
+    "arrival_time": "08:00",
+    "departure_airport": {
+        "city": "San Jose",
+        "code": "SJC",
+        "id": "61849d3f4367d925b16ff24b",
+        "name": "San Jose International Airport"
+    },
+    "departure_date": "Sun, 09 Jan 2022 00:00:00 GMT",
+    "departure_time": "07:00",
+    "flight_num": "AA3457",
+    "flight_status": "scheduled",
+    "id": "61a5ae2a46401bf4c54c8c1e",
+    "price": "40.00",
+    "remaining_seats": 90,
+    "seat_chart": {
+        "aisle": [
+            "1A"
+        ],
+        "middle": [
+            "1B"
+        ],
+        "window": [
+            "1C"
+        ]
+    },
+    "seat_price": {
+        "aisle": 3,
+        "middle": 0,
+        "window": 5
+    },
+    "seats": {
+        "aisle": 30,
+        "middle": 30,
+        "window": 30
+    }
 }</t>
   </si>
 </sst>
@@ -1591,10 +1693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137CDCEF-55E1-8E4F-A1FE-9A17006F53F5}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="144" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="144" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11"/>
@@ -1610,7 +1712,7 @@
     <col min="10" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="12">
+    <row r="1" spans="1:10" ht="12">
       <c r="B1" s="6" t="s">
         <v>34</v>
       </c>
@@ -1636,7 +1738,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -1657,7 +1759,7 @@
       </c>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="295">
+    <row r="3" spans="1:10" ht="295">
       <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1680,7 +1782,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="156">
+    <row r="4" spans="1:10" ht="156">
       <c r="C4" s="6" t="s">
         <v>8</v>
       </c>
@@ -1703,7 +1805,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="48">
+    <row r="6" spans="1:10" ht="48">
       <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
@@ -1726,7 +1828,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="84">
+    <row r="7" spans="1:10" ht="84">
       <c r="C7" s="6" t="s">
         <v>14</v>
       </c>
@@ -1746,7 +1848,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="84">
+    <row r="8" spans="1:10" ht="84">
       <c r="C8" s="6" t="s">
         <v>74</v>
       </c>
@@ -1763,7 +1865,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="144">
+    <row r="9" spans="1:10" ht="144">
       <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
@@ -1789,7 +1891,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="409.6">
+    <row r="10" spans="1:10" ht="409.6">
       <c r="C10" s="6" t="s">
         <v>18</v>
       </c>
@@ -1808,8 +1910,11 @@
       <c r="H10" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="409.6">
+      <c r="I10" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="409.6">
       <c r="C11" s="6" t="s">
         <v>38</v>
       </c>
@@ -1825,8 +1930,12 @@
       <c r="G11" s="7" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="I11" s="7"/>
+      <c r="J11" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="6" t="s">
         <v>41</v>
       </c>
@@ -1837,7 +1946,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="409.6">
+    <row r="13" spans="1:10" ht="409.6">
       <c r="C13" s="6" t="s">
         <v>48</v>
       </c>
@@ -1854,7 +1963,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="192">
+    <row r="14" spans="1:10" ht="192">
       <c r="C14" s="6" t="s">
         <v>49</v>
       </c>
@@ -1874,7 +1983,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="350">
+    <row r="16" spans="1:10" ht="350">
       <c r="A16" s="6" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
changes for booking json error
</commit_message>
<xml_diff>
--- a/API_documentation.xlsx
+++ b/API_documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhitholar/college_work/cmpe202/team_project/team-project-team_techies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F58AD4-B93B-3E43-AAD9-455DF8068499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C8C283-C5A9-D44A-914A-D87B7CA9EB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11640" yWindow="-20260" windowWidth="28800" windowHeight="18040" xr2:uid="{AB8BB195-AD8F-664F-886C-5E9BDDAF898A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{AB8BB195-AD8F-664F-886C-5E9BDDAF898A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="108">
   <si>
     <t>Methid</t>
   </si>
@@ -1233,6 +1233,76 @@
         "window": 30
     }
 }</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "booked_price": 100,
+        "booking_history": "booked",
+        "booking_num": "#YX6X822728XO",
+        "flight_oid": {
+            "aircraft": {
+                "id": "61a5aac8b657dbd44f933bb9",
+                "name": "Airbus A320"
+            },
+            "arrival_airport": {
+                "city": "San Francisco",
+                "code": "SFO",
+                "id": "61849d5f4367d925b16ff24c",
+                "name": "San Francisco International Airport"
+            },
+            "arrival_date": "Sun, 09 Jan 2022 00:00:00 GMT",
+            "arrival_time": "08:00",
+            "departure_airport": {
+                "city": "San Jose",
+                "code": "SJC",
+                "id": "61849d3f4367d925b16ff24b",
+                "name": "San Jose International Airport"
+            },
+            "departure_date": "Sun, 09 Jan 2022 00:00:00 GMT",
+            "departure_time": "07:00",
+            "flight_num": "AA3457",
+            "flight_status": "scheduled",
+            "id": "61a5ae2a46401bf4c54c8c1e",
+            "price": "100.00",
+            "remaining_seats": 87,
+            "seat_chart": {
+                "aisle": [
+                    "1A"
+                ],
+                "middle": [
+                    "1B"
+                ],
+                "window": [
+                    "1C"
+                ]
+            },
+            "seat_price": {
+                "aisle": 3,
+                "middle": 0,
+                "window": 5
+            },
+            "seats": {
+                "aisle": 30,
+                "middle": 30,
+                "window": 30
+            }
+        },
+        "flight_status": "scheduled",
+        "id": "61a5b47af22ceb8caa49833f",
+        "mileage_points_earned": 18.0,
+        "payment": {
+            "cash": 90,
+            "reward_points_used": 10
+        },
+        "seat_num": null,
+        "seat_price": null,
+        "seat_type": null,
+        "traveller_details": {
+            "name": "xyz"
+        }
+    }
+]</t>
   </si>
 </sst>
 </file>
@@ -1695,8 +1765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137CDCEF-55E1-8E4F-A1FE-9A17006F53F5}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="144" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="144" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11"/>
@@ -2028,6 +2098,9 @@
       <c r="H17" s="6" t="s">
         <v>29</v>
       </c>
+      <c r="I17" s="7" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="409.6">
       <c r="C19" s="6" t="s">

</xml_diff>